<commit_message>
Convert machine array to Graph nodes
</commit_message>
<xml_diff>
--- a/data/Machines_Data.xlsx
+++ b/data/Machines_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\MSTS_FJSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F55B7D-630E-4AF4-9430-003DFCE56DEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11D33F0-51BB-418C-8F4A-4838E25F19CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -453,11 +453,11 @@
       </c>
       <c r="D2" s="1">
         <f ca="1">RANDBETWEEN(50,150)/100</f>
-        <v>1.5</v>
+        <v>1.06</v>
       </c>
       <c r="E2" s="1">
         <f ca="1">RANDBETWEEN(50,150)/100</f>
-        <v>1.01</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -472,11 +472,11 @@
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:E5" ca="1" si="0">RANDBETWEEN(50,150)/100</f>
-        <v>1.47</v>
+        <v>0.68</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -491,11 +491,11 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.01</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -510,11 +510,11 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>1.28</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.01</v>
+        <v>0.68</v>
       </c>
     </row>
   </sheetData>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3673E1-565D-41DE-9737-D9BBE2EAEAF2}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,15 +556,15 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:E5" ca="1" si="0">ROUND(RAND()*100,0)</f>
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -572,19 +572,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B5" ca="1" si="1">ROUND(RAND()*100,0)</f>
-        <v>69</v>
+        <f ca="1">C2</f>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -592,19 +592,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <f ca="1">D2</f>
+        <v>79</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <f ca="1">D3</f>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -612,16 +612,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <f ca="1">E2</f>
+        <v>58</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <f ca="1">E3</f>
+        <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <f ca="1">E4</f>
+        <v>79</v>
       </c>
       <c r="E5">
         <v>0</v>

</xml_diff>